<commit_message>
added tables stw occupation
</commit_message>
<xml_diff>
--- a/src/shiny-dashboard/stwFluid/stw_occupations_tables.xlsx
+++ b/src/shiny-dashboard/stwFluid/stw_occupations_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah McDonald\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70051F86-DB71-4D97-A5AB-C773E7BF5DA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E07DED0-8F33-4C4A-977F-9BE7059C9208}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{814E42C7-6095-4C0D-B056-D340EFD0D8EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="490">
   <si>
     <t>Occupation Name</t>
   </si>
@@ -1244,9 +1244,6 @@
     <t>47-4011.01</t>
   </si>
   <si>
-    <t xml:space="preserve"> 11-3051</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Compliance Officers </t>
     </r>
@@ -1591,6 +1588,12 @@
   </si>
   <si>
     <t>53-7062.04</t>
+  </si>
+  <si>
+    <t>soc_stw</t>
+  </si>
+  <si>
+    <t>onet_stw</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1771,6 +1774,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2086,15 +2092,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399BBFE0-6717-4236-AC1A-E8604140EC5F}">
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2104,8 +2114,14 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D1" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2115,8 +2131,14 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -2126,8 +2148,14 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -2137,8 +2165,14 @@
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2148,8 +2182,14 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -2159,8 +2199,14 @@
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -2170,8 +2216,14 @@
       <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -2181,8 +2233,14 @@
       <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -2192,8 +2250,14 @@
       <c r="C9" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -2203,8 +2267,14 @@
       <c r="C10" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -2214,8 +2284,14 @@
       <c r="C11" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -2225,8 +2301,14 @@
       <c r="C12" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
@@ -2236,8 +2318,14 @@
       <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -2247,8 +2335,14 @@
       <c r="C14" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>40</v>
       </c>
@@ -2258,8 +2352,14 @@
       <c r="C15" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>43</v>
       </c>
@@ -2269,8 +2369,14 @@
       <c r="C16" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>46</v>
       </c>
@@ -2280,8 +2386,14 @@
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
@@ -2291,8 +2403,14 @@
       <c r="C18" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
         <v>52</v>
       </c>
@@ -2302,8 +2420,14 @@
       <c r="C19" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
         <v>55</v>
       </c>
@@ -2313,8 +2437,14 @@
       <c r="C20" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>58</v>
       </c>
@@ -2324,8 +2454,14 @@
       <c r="C21" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>61</v>
       </c>
@@ -2335,8 +2471,14 @@
       <c r="C22" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
         <v>64</v>
       </c>
@@ -2346,8 +2488,14 @@
       <c r="C23" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
         <v>67</v>
       </c>
@@ -2357,8 +2505,14 @@
       <c r="C24" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
         <v>70</v>
       </c>
@@ -2368,8 +2522,14 @@
       <c r="C25" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>73</v>
       </c>
@@ -2379,8 +2539,14 @@
       <c r="C26" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>76</v>
       </c>
@@ -2390,8 +2556,14 @@
       <c r="C27" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
         <v>79</v>
       </c>
@@ -2401,8 +2573,14 @@
       <c r="C28" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
         <v>82</v>
       </c>
@@ -2412,8 +2590,14 @@
       <c r="C29" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
         <v>85</v>
       </c>
@@ -2423,8 +2607,14 @@
       <c r="C30" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>88</v>
       </c>
@@ -2434,8 +2624,14 @@
       <c r="C31" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>91</v>
       </c>
@@ -2445,8 +2641,14 @@
       <c r="C32" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
         <v>94</v>
       </c>
@@ -2456,8 +2658,14 @@
       <c r="C33" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="5" t="s">
         <v>97</v>
       </c>
@@ -2467,8 +2675,14 @@
       <c r="C34" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="5" t="s">
         <v>100</v>
       </c>
@@ -2478,8 +2692,14 @@
       <c r="C35" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="5" t="s">
         <v>103</v>
       </c>
@@ -2489,8 +2709,14 @@
       <c r="C36" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>106</v>
       </c>
@@ -2500,8 +2726,14 @@
       <c r="C37" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="5" t="s">
         <v>109</v>
       </c>
@@ -2511,8 +2743,14 @@
       <c r="C38" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
         <v>112</v>
       </c>
@@ -2522,8 +2760,14 @@
       <c r="C39" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="5" t="s">
         <v>115</v>
       </c>
@@ -2533,8 +2777,14 @@
       <c r="C40" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="5" t="s">
         <v>118</v>
       </c>
@@ -2544,8 +2794,14 @@
       <c r="C41" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>121</v>
       </c>
@@ -2555,8 +2811,14 @@
       <c r="C42" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="5" t="s">
         <v>124</v>
       </c>
@@ -2566,8 +2828,14 @@
       <c r="C43" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="5" t="s">
         <v>127</v>
       </c>
@@ -2577,8 +2845,14 @@
       <c r="C44" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>130</v>
       </c>
@@ -2588,8 +2862,14 @@
       <c r="C45" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="5" t="s">
         <v>133</v>
       </c>
@@ -2599,8 +2879,14 @@
       <c r="C46" s="4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
         <v>136</v>
       </c>
@@ -2610,8 +2896,14 @@
       <c r="C47" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="5" t="s">
         <v>139</v>
       </c>
@@ -2621,8 +2913,14 @@
       <c r="C48" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>142</v>
       </c>
@@ -2632,8 +2930,14 @@
       <c r="C49" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="5" t="s">
         <v>145</v>
       </c>
@@ -2643,8 +2947,14 @@
       <c r="C50" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>148</v>
       </c>
@@ -2654,8 +2964,14 @@
       <c r="C51" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>151</v>
       </c>
@@ -2665,8 +2981,14 @@
       <c r="C52" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
         <v>154</v>
       </c>
@@ -2676,8 +2998,14 @@
       <c r="C53" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
         <v>157</v>
       </c>
@@ -2687,8 +3015,14 @@
       <c r="C54" s="4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>160</v>
       </c>
@@ -2698,8 +3032,14 @@
       <c r="C55" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="5" t="s">
         <v>163</v>
       </c>
@@ -2709,8 +3049,14 @@
       <c r="C56" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="5" t="s">
         <v>166</v>
       </c>
@@ -2720,8 +3066,14 @@
       <c r="C57" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="5" t="s">
         <v>169</v>
       </c>
@@ -2731,8 +3083,14 @@
       <c r="C58" s="4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>172</v>
       </c>
@@ -2742,8 +3100,14 @@
       <c r="C59" s="4" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>175</v>
       </c>
@@ -2753,8 +3117,14 @@
       <c r="C60" s="4" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>178</v>
       </c>
@@ -2764,8 +3134,14 @@
       <c r="C61" s="4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
         <v>181</v>
       </c>
@@ -2775,8 +3151,14 @@
       <c r="C62" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>184</v>
       </c>
@@ -2786,8 +3168,14 @@
       <c r="C63" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>187</v>
       </c>
@@ -2797,8 +3185,14 @@
       <c r="C64" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
         <v>190</v>
       </c>
@@ -2808,8 +3202,14 @@
       <c r="C65" s="4" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="5" t="s">
         <v>193</v>
       </c>
@@ -2819,8 +3219,14 @@
       <c r="C66" s="4" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="5" t="s">
         <v>196</v>
       </c>
@@ -2830,8 +3236,14 @@
       <c r="C67" s="4" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="5" t="s">
         <v>199</v>
       </c>
@@ -2841,8 +3253,14 @@
       <c r="C68" s="4" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="5" t="s">
         <v>202</v>
       </c>
@@ -2852,8 +3270,14 @@
       <c r="C69" s="4" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="5" t="s">
         <v>205</v>
       </c>
@@ -2863,8 +3287,14 @@
       <c r="C70" s="4" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="5" t="s">
         <v>208</v>
       </c>
@@ -2874,8 +3304,14 @@
       <c r="C71" s="4" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="5" t="s">
         <v>211</v>
       </c>
@@ -2885,8 +3321,14 @@
       <c r="C72" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="5" t="s">
         <v>214</v>
       </c>
@@ -2896,8 +3338,14 @@
       <c r="C73" s="4" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="5" t="s">
         <v>217</v>
       </c>
@@ -2907,8 +3355,14 @@
       <c r="C74" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="5" t="s">
         <v>220</v>
       </c>
@@ -2918,8 +3372,14 @@
       <c r="C75" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="5" t="s">
         <v>223</v>
       </c>
@@ -2929,8 +3389,14 @@
       <c r="C76" s="4" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="5" t="s">
         <v>226</v>
       </c>
@@ -2940,8 +3406,14 @@
       <c r="C77" s="4" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="5" t="s">
         <v>229</v>
       </c>
@@ -2951,8 +3423,14 @@
       <c r="C78" s="4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="5" t="s">
         <v>232</v>
       </c>
@@ -2962,8 +3440,14 @@
       <c r="C79" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="5" t="s">
         <v>235</v>
       </c>
@@ -2973,8 +3457,14 @@
       <c r="C80" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="5" t="s">
         <v>238</v>
       </c>
@@ -2984,8 +3474,14 @@
       <c r="C81" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="5" t="s">
         <v>241</v>
       </c>
@@ -2995,8 +3491,14 @@
       <c r="C82" s="4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="5" t="s">
         <v>244</v>
       </c>
@@ -3006,8 +3508,14 @@
       <c r="C83" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="5" t="s">
         <v>247</v>
       </c>
@@ -3017,8 +3525,14 @@
       <c r="C84" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="5" t="s">
         <v>250</v>
       </c>
@@ -3028,8 +3542,14 @@
       <c r="C85" s="4" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>253</v>
       </c>
@@ -3039,8 +3559,14 @@
       <c r="C86" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>256</v>
       </c>
@@ -3050,8 +3576,14 @@
       <c r="C87" s="4" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="5" t="s">
         <v>259</v>
       </c>
@@ -3061,8 +3593,14 @@
       <c r="C88" s="4" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="5" t="s">
         <v>262</v>
       </c>
@@ -3072,8 +3610,14 @@
       <c r="C89" s="4" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="5" t="s">
         <v>265</v>
       </c>
@@ -3083,8 +3627,14 @@
       <c r="C90" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="5" t="s">
         <v>268</v>
       </c>
@@ -3094,8 +3644,14 @@
       <c r="C91" s="4" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="5" t="s">
         <v>271</v>
       </c>
@@ -3105,8 +3661,14 @@
       <c r="C92" s="4" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="5" t="s">
         <v>274</v>
       </c>
@@ -3116,8 +3678,14 @@
       <c r="C93" s="4" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="5" t="s">
         <v>277</v>
       </c>
@@ -3127,8 +3695,14 @@
       <c r="C94" s="4" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="5" t="s">
         <v>280</v>
       </c>
@@ -3138,8 +3712,14 @@
       <c r="C95" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="5" t="s">
         <v>283</v>
       </c>
@@ -3149,8 +3729,14 @@
       <c r="C96" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="5" t="s">
         <v>286</v>
       </c>
@@ -3160,8 +3746,14 @@
       <c r="C97" s="4" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="5" t="s">
         <v>289</v>
       </c>
@@ -3171,8 +3763,14 @@
       <c r="C98" s="4" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="5" t="s">
         <v>292</v>
       </c>
@@ -3182,8 +3780,14 @@
       <c r="C99" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="5" t="s">
         <v>295</v>
       </c>
@@ -3193,8 +3797,14 @@
       <c r="C100" s="4" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>298</v>
       </c>
@@ -3204,8 +3814,14 @@
       <c r="C101" s="4" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="5" t="s">
         <v>301</v>
       </c>
@@ -3215,8 +3831,14 @@
       <c r="C102" s="4" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="5" t="s">
         <v>304</v>
       </c>
@@ -3226,8 +3848,14 @@
       <c r="C103" s="4" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="5" t="s">
         <v>307</v>
       </c>
@@ -3237,8 +3865,14 @@
       <c r="C104" s="4" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="5" t="s">
         <v>310</v>
       </c>
@@ -3248,8 +3882,14 @@
       <c r="C105" s="4" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="5" t="s">
         <v>313</v>
       </c>
@@ -3259,8 +3899,14 @@
       <c r="C106" s="4" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="5" t="s">
         <v>316</v>
       </c>
@@ -3270,8 +3916,14 @@
       <c r="C107" s="4" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="5" t="s">
         <v>319</v>
       </c>
@@ -3281,8 +3933,14 @@
       <c r="C108" s="4" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="5" t="s">
         <v>322</v>
       </c>
@@ -3292,8 +3950,14 @@
       <c r="C109" s="4" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="5" t="s">
         <v>325</v>
       </c>
@@ -3303,8 +3967,14 @@
       <c r="C110" s="4" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="5" t="s">
         <v>328</v>
       </c>
@@ -3314,8 +3984,14 @@
       <c r="C111" s="4" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="5" t="s">
         <v>331</v>
       </c>
@@ -3325,8 +4001,14 @@
       <c r="C112" s="4" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="5" t="s">
         <v>334</v>
       </c>
@@ -3336,8 +4018,14 @@
       <c r="C113" s="4" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="5" t="s">
         <v>337</v>
       </c>
@@ -3347,8 +4035,14 @@
       <c r="C114" s="4" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="5" t="s">
         <v>340</v>
       </c>
@@ -3358,8 +4052,14 @@
       <c r="C115" s="4" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="5" t="s">
         <v>343</v>
       </c>
@@ -3369,8 +4069,14 @@
       <c r="C116" s="4" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A117" s="5" t="s">
         <v>346</v>
       </c>
@@ -3380,8 +4086,14 @@
       <c r="C117" s="4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="5" t="s">
         <v>349</v>
       </c>
@@ -3391,8 +4103,14 @@
       <c r="C118" s="4" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="8"/>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
@@ -3405,10 +4123,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDDD8C5-EB54-42EE-B2A1-097EE7AED7CB}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3417,7 +4135,7 @@
     <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="89" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="89" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>353</v>
       </c>
@@ -3427,74 +4145,116 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D1" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>391</v>
+      <c r="B2" s="11">
+        <v>420700</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="65.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="65.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>391</v>
+      <c r="B3" s="11">
+        <v>420700</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>391</v>
+      <c r="B4" s="11">
+        <v>420700</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>391</v>
+      <c r="B5" s="11">
+        <v>420700</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="65.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="65.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>391</v>
+      <c r="B6" s="11">
+        <v>420700</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="65.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="65.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>391</v>
+      <c r="B7" s="11">
+        <v>420700</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="10" t="s">
         <v>366</v>
       </c>
@@ -3504,8 +4264,14 @@
       <c r="C8" s="4" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>369</v>
       </c>
@@ -3515,8 +4281,14 @@
       <c r="C9" s="9" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>371</v>
       </c>
@@ -3526,8 +4298,14 @@
       <c r="C10" s="4" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>374</v>
       </c>
@@ -3537,8 +4315,14 @@
       <c r="C11" s="4" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>376</v>
       </c>
@@ -3548,8 +4332,14 @@
       <c r="C12" s="4" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>379</v>
       </c>
@@ -3559,8 +4349,14 @@
       <c r="C13" s="9" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>381</v>
       </c>
@@ -3570,8 +4366,14 @@
       <c r="C14" s="4" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="65.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="65.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>384</v>
       </c>
@@ -3581,8 +4383,14 @@
       <c r="C15" s="4" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>386</v>
       </c>
@@ -3592,8 +4400,14 @@
       <c r="C16" s="4" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>389</v>
       </c>
@@ -3602,6 +4416,12 @@
       </c>
       <c r="C17" s="4" t="s">
         <v>390</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3612,15 +4432,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB929547-5320-48B5-91F7-C37867CEFFD1}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="89" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="89" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>353</v>
       </c>
@@ -3630,467 +4450,725 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D1" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>392</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
+      <c r="B3" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
+      <c r="B4" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
+      <c r="B5" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="10" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
+      <c r="B6" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C9" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>408</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="10" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="10" t="s">
+      <c r="B11" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="10" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="10" t="s">
+      <c r="B12" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="5" t="s">
+      <c r="B16" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="C16" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>425</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>425</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="5" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="C19" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="5" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="5" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="5" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="5" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>440</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="5" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="14" t="s">
         <v>442</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="C24" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="5" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="5" t="s">
+      <c r="B25" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="5" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="5" t="s">
+      <c r="B26" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="5" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="5" t="s">
+      <c r="B27" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="5" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="5" t="s">
+      <c r="B28" s="14" t="s">
         <v>451</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="C28" s="9" t="s">
         <v>452</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="5" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="5" t="s">
+      <c r="B29" s="14" t="s">
+        <v>451</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>452</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="5" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="5" t="s">
+      <c r="B30" s="14" t="s">
         <v>456</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="C30" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="5" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="5" t="s">
+      <c r="B31" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>457</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="5" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="5" t="s">
+      <c r="B32" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="C32" s="9" t="s">
         <v>462</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="5" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="5" t="s">
+      <c r="B33" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>462</v>
-      </c>
-      <c r="C33" s="9" t="s">
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="5" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="5" t="s">
+      <c r="B34" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>462</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="5" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="5" t="s">
+      <c r="B35" s="14" t="s">
         <v>468</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="C35" s="9" t="s">
         <v>469</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="5" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="5" t="s">
+      <c r="B36" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>469</v>
-      </c>
-      <c r="C36" s="9" t="s">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="5" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="5" t="s">
+      <c r="B37" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="B37" s="14" t="s">
-        <v>469</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="5" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="5" t="s">
+      <c r="B38" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>469</v>
-      </c>
-      <c r="C38" s="9" t="s">
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="5" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="5" t="s">
+      <c r="B39" s="14" t="s">
         <v>477</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="C39" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="5" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="5" t="s">
+      <c r="B40" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>478</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="5" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="5" t="s">
+      <c r="B41" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="B41" s="14" t="s">
-        <v>478</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="5" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="5" t="s">
+      <c r="B42" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="C42" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="5" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="5" t="s">
+      <c r="B43" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="B43" s="14" t="s">
-        <v>485</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>488</v>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>